<commit_message>
Arbeiten SW & SW zum 24.03.2020
</commit_message>
<xml_diff>
--- a/Allgemein/Einkaufsliste.xlsx
+++ b/Allgemein/Einkaufsliste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swagn\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swagn\OneDrive\Desktop\Projecte\Workshop\Indicator.git\Allgemein\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30A283E-2434-4E95-8968-8F57D6906834}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A46D69-007E-4D77-8C5F-953327802943}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Einkaufsliste:</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>MSTBA 2,5/12-G - 1757569</t>
+  </si>
+  <si>
+    <t>MSTBA12</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:M16"/>
+  <dimension ref="B3:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,7 +480,7 @@
     <col min="10" max="10" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -503,7 +509,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
@@ -526,7 +532,7 @@
         <v>1923898</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2</v>
       </c>
@@ -549,106 +555,115 @@
         <v>1923908</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="O7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I8" s="3">
         <v>1612471</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10">
         <v>5</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11">
         <v>6</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="1" t="s">
+      <c r="K11" s="4"/>
+      <c r="L11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12">
         <v>7</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L10" r:id="rId1" xr:uid="{7391F758-8D5D-446A-9C97-54119C8ED310}"/>
-    <hyperlink ref="F11" r:id="rId2" xr:uid="{41547C99-91E5-477C-904A-B5BD8F702738}"/>
+    <hyperlink ref="L11" r:id="rId1" xr:uid="{7391F758-8D5D-446A-9C97-54119C8ED310}"/>
+    <hyperlink ref="F12" r:id="rId2" xr:uid="{41547C99-91E5-477C-904A-B5BD8F702738}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>